<commit_message>
add show all func
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Documents\_Programming\Python\stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A235C9-3377-4944-83B6-F4039803A4E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B487AC1-6194-4FA4-88BB-94DF711DAEFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6165" yWindow="3165" windowWidth="19965" windowHeight="11145" xr2:uid="{1E6380F2-32CF-4CDB-84C9-9C534D2AC723}"/>
   </bookViews>
@@ -457,7 +457,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15.75"/>
@@ -649,7 +649,7 @@
         <v>200</v>
       </c>
       <c r="E11">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:6">

</xml_diff>